<commit_message>
Update patient - Pritee
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -1,27 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hristo.tentchev.OFFICE-SF\Desktop\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptang\git\DieticianAPI\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4EC5A2-F03E-4EE0-BA2A-48B1DD28B943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="PriteeUpt" sheetId="2" r:id="rId2"/>
+    <sheet name="Sudha" sheetId="3" r:id="rId3"/>
+    <sheet name="Pritee" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="S-Negative" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
   <si>
     <t>password</t>
   </si>
@@ -77,19 +82,67 @@
     <t>Vegan</t>
   </si>
   <si>
-    <t>1989-02-02</t>
-  </si>
-  <si>
-    <t>2909909909</t>
-  </si>
-  <si>
     <t>1985-05-01</t>
+  </si>
+  <si>
+    <t>Kimy</t>
+  </si>
+  <si>
+    <t>2909909924</t>
+  </si>
+  <si>
+    <t>johm.kimy@gmail.com</t>
+  </si>
+  <si>
+    <t>1985-05-11</t>
+  </si>
+  <si>
+    <t>3456789128</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Alex.kim@gmail.com</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>julia.smith@gmail.com</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>a.bob@gmail.com</t>
+  </si>
+  <si>
+    <t>Walnut</t>
+  </si>
+  <si>
+    <t>NonVeg</t>
+  </si>
+  <si>
+    <t>2001-01-01</t>
+  </si>
+  <si>
+    <t>2912349909</t>
+  </si>
+  <si>
+    <t>2005-06-06</t>
+  </si>
+  <si>
+    <t>8736345566</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -102,36 +155,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="10"/>
-      <u val="single"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="10"/>
-      <u val="single"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <color theme="10"/>
-      <u val="single"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -151,84 +204,42 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
-      <alignment vertical="bottom"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
-      <alignment/>
-      <protection/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,19 +553,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" width="26.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -570,7 +581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -580,156 +591,416 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" display="mailsudhamaha@gmail.com" r:id="rId1"/>
-    <hyperlink ref="B3" display="pranithareddy83@gmail.com" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0" defaultColWidth="9.140625"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1" style="4"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1" style="4"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1" style="4"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1" style="4"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1" style="4"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1" bestFit="1" style="4"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="14.1796875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="30.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="3"/>
+    <col min="6" max="6" width="19.7265625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="1" s="4">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4">
-        <v>2482482481</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>18</v>
+      <c r="G2" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" display="johm.kim@gmail.com" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="1" max="7" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>20</v>
+      <c r="G2" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" display="johm.kim@gmail.com" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="johm.kim@gmail.com" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{590DEFB5-1B54-45BD-B92B-1BA3F63F1929}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="8">
+        <v>9078564321</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="9">
+        <v>31970</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74B6FF6-2156-4A19-AE5F-89F9475F9001}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+    <col min="4" max="5" width="20.81640625" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="8">
+        <v>7892456540</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="9">
+        <v>30418</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>